<commit_message>
DOMA-2027 DOMA-2028 template improved
</commit_message>
<xml_diff>
--- a/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
+++ b/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
@@ -28,34 +28,34 @@
     <t>Почта</t>
   </si>
   <si>
-    <t>{d.contacts[I].name}</t>
-  </si>
-  <si>
-    <t>{d.contacts[I].address}</t>
-  </si>
-  <si>
-    <t>{d.contacts[I].unitName}</t>
-  </si>
-  <si>
-    <t>{d.contacts[I].phone}</t>
-  </si>
-  <si>
-    <t>{d.contacts[I].email}</t>
-  </si>
-  <si>
-    <t>{d.contacts[I+1].name}</t>
-  </si>
-  <si>
-    <t>{d.contacts[I+1].address}</t>
-  </si>
-  <si>
-    <t>{d.contacts[I+1].unitName}</t>
-  </si>
-  <si>
-    <t>{d.contacts[I+1].phone}</t>
-  </si>
-  <si>
-    <t>{d.contacts[I+1].email}</t>
+    <t>{d.contacts[i].name}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i].address}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i].unitName}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i].phone}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i].email}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i+1].name}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i+1].address}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i+1].unitName}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i+1].phone}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i+1].email}</t>
   </si>
 </sst>
 </file>
@@ -65,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -77,12 +77,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +98,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -162,13 +174,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -191,6 +203,7 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1254,17 +1267,15 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="37.8906" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.4531" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88281" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.4531" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85156" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1719" style="1" customWidth="1"/>
     <col min="6" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
DOMA-2542 Localization for Excel template (contacts)
</commit_message>
<xml_diff>
--- a/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
+++ b/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Контакты" sheetId="1" r:id="rId4"/>
+    <sheet name="{d.i18n.sheetName}" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -13,19 +13,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
-    <t>Имя</t>
-  </si>
-  <si>
-    <t>Адрес</t>
-  </si>
-  <si>
-    <t>Квартира</t>
-  </si>
-  <si>
-    <t>Телефон</t>
-  </si>
-  <si>
-    <t>Почта</t>
+    <t>{d.i18n.name}</t>
+  </si>
+  <si>
+    <t>{d.i18n.address}</t>
+  </si>
+  <si>
+    <t>{d.i18n.unitName}</t>
+  </si>
+  <si>
+    <t>{d.i18n.phone}</t>
+  </si>
+  <si>
+    <t>{d.i18n.email}</t>
   </si>
   <si>
     <t>{d.contacts[i].name}</t>

</xml_diff>

<commit_message>
Revert "DOMA-2542 Localization for Excel template (contacts)"
This reverts commit fa8ed8a169bfd266ae1c45f6e511747f57ff74a1.
</commit_message>
<xml_diff>
--- a/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
+++ b/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="{d.i18n.sheetName}" sheetId="1" r:id="rId4"/>
+    <sheet name="Контакты" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -13,19 +13,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
-    <t>{d.i18n.name}</t>
-  </si>
-  <si>
-    <t>{d.i18n.address}</t>
-  </si>
-  <si>
-    <t>{d.i18n.unitName}</t>
-  </si>
-  <si>
-    <t>{d.i18n.phone}</t>
-  </si>
-  <si>
-    <t>{d.i18n.email}</t>
+    <t>Имя</t>
+  </si>
+  <si>
+    <t>Адрес</t>
+  </si>
+  <si>
+    <t>Квартира</t>
+  </si>
+  <si>
+    <t>Телефон</t>
+  </si>
+  <si>
+    <t>Почта</t>
   </si>
   <si>
     <t>{d.contacts[i].name}</t>

</xml_diff>

<commit_message>
DOMA-3097 add unitType field to contact exporting fields
</commit_message>
<xml_diff>
--- a/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
+++ b/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>{d.i18n.name}</t>
   </si>
@@ -28,6 +28,9 @@
     <t>{d.i18n.email}</t>
   </si>
   <si>
+    <t>{d.i18n.unitType}</t>
+  </si>
+  <si>
     <t>{d.contacts[i].name}</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t>{d.contacts[i].email}</t>
   </si>
   <si>
+    <t>{d.contacts[I].unitType}</t>
+  </si>
+  <si>
     <t>{d.contacts[i+1].name}</t>
   </si>
   <si>
@@ -56,6 +62,9 @@
   </si>
   <si>
     <t>{d.contacts[i+1].email}</t>
+  </si>
+  <si>
+    <t>{d.contacts[I+1].unitType}</t>
   </si>
 </sst>
 </file>
@@ -108,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -161,13 +170,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -181,6 +277,33 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -204,6 +327,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1265,7 +1389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1273,10 +1397,10 @@
   <cols>
     <col min="1" max="1" width="37.8516" style="1" customWidth="1"/>
     <col min="2" max="2" width="41.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1875" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1719" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="19.1719" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1295,40 +1419,105 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="39" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>11</v>
       </c>
     </row>
     <row r="3" ht="39" customHeight="1">
       <c r="A3" t="s" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s" s="4">
-        <v>14</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F3" t="s" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>

</xml_diff>

<commit_message>
DOMA-3097 review fixes for contact export
</commit_message>
<xml_diff>
--- a/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
+++ b/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
@@ -22,15 +22,15 @@
     <t>{d.i18n.unitName}</t>
   </si>
   <si>
+    <t>{d.i18n.unitType}</t>
+  </si>
+  <si>
     <t>{d.i18n.phone}</t>
   </si>
   <si>
     <t>{d.i18n.email}</t>
   </si>
   <si>
-    <t>{d.i18n.unitType}</t>
-  </si>
-  <si>
     <t>{d.contacts[i].name}</t>
   </si>
   <si>
@@ -40,15 +40,15 @@
     <t>{d.contacts[i].unitName}</t>
   </si>
   <si>
+    <t>{d.contacts[I].unitType}</t>
+  </si>
+  <si>
     <t>{d.contacts[i].phone}</t>
   </si>
   <si>
     <t>{d.contacts[i].email}</t>
   </si>
   <si>
-    <t>{d.contacts[I].unitType}</t>
-  </si>
-  <si>
     <t>{d.contacts[i+1].name}</t>
   </si>
   <si>
@@ -58,13 +58,13 @@
     <t>{d.contacts[i+1].unitName}</t>
   </si>
   <si>
+    <t>{d.contacts[I+1].unitType}</t>
+  </si>
+  <si>
     <t>{d.contacts[i+1].phone}</t>
   </si>
   <si>
     <t>{d.contacts[i+1].email}</t>
-  </si>
-  <si>
-    <t>{d.contacts[I+1].unitType}</t>
   </si>
 </sst>
 </file>
@@ -1397,9 +1397,9 @@
   <cols>
     <col min="1" max="1" width="37.8516" style="1" customWidth="1"/>
     <col min="2" max="2" width="41.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="19.1719" style="1" customWidth="1"/>
+    <col min="3" max="4" width="19.1719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1719" style="1" customWidth="1"/>
     <col min="7" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1467,56 +1467,56 @@
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="10"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="10"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="10"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="10"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="10"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DOMA-3372 The `role` field was added to excel export
</commit_message>
<xml_diff>
--- a/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
+++ b/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>{d.i18n.name}</t>
   </si>
@@ -31,6 +31,9 @@
     <t>{d.i18n.email}</t>
   </si>
   <si>
+    <t>{d.i18n.role}</t>
+  </si>
+  <si>
     <t>{d.contacts[i].name}</t>
   </si>
   <si>
@@ -49,6 +52,9 @@
     <t>{d.contacts[i].email}</t>
   </si>
   <si>
+    <t>{d.contacts[i].role}</t>
+  </si>
+  <si>
     <t>{d.contacts[i+1].name}</t>
   </si>
   <si>
@@ -65,6 +71,9 @@
   </si>
   <si>
     <t>{d.contacts[i+1].email}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i+1].role}</t>
   </si>
 </sst>
 </file>
@@ -117,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -170,100 +179,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -277,33 +199,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -327,7 +222,6 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1389,7 +1283,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1399,8 +1293,8 @@
     <col min="2" max="2" width="41.5" style="1" customWidth="1"/>
     <col min="3" max="4" width="19.1719" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1719" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="7" width="19.1719" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1422,102 +1316,55 @@
       <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" ht="39" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>13</v>
       </c>
     </row>
     <row r="3" ht="39" customHeight="1">
       <c r="A3" t="s" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s" s="4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="G3" t="s" s="4">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>

</xml_diff>

<commit_message>
feat(condo): DOMA-4473 initialize feat verifying contact
</commit_message>
<xml_diff>
--- a/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
+++ b/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
@@ -1,17 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25811"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A7B2708-B096-4C84-AF74-F5CE9C2602FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="{d.i18n.sheetName}" sheetId="1" r:id="rId4"/>
+    <sheet name="{d.i18n.sheetName}" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>{d.i18n.isVerified}</t>
+  </si>
   <si>
     <t>{d.i18n.name}</t>
   </si>
@@ -34,6 +54,9 @@
     <t>{d.i18n.role}</t>
   </si>
   <si>
+    <t>{d.contacts[i].isVerified}</t>
+  </si>
+  <si>
     <t>{d.contacts[i].name}</t>
   </si>
   <si>
@@ -53,6 +76,9 @@
   </si>
   <si>
     <t>{d.contacts[i].role}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i+1].isVerified}</t>
   </si>
   <si>
     <t>{d.contacts[i+1].name}</t>
@@ -79,28 +105,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -181,54 +194,101 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -430,7 +490,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -449,7 +509,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -479,7 +539,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -505,7 +565,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -531,7 +591,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -557,7 +617,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -583,7 +643,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -609,7 +669,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -635,7 +695,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -661,7 +721,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -687,7 +747,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -700,9 +760,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -719,7 +785,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -738,7 +804,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -764,7 +830,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -790,7 +856,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -816,7 +882,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -842,7 +908,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -868,7 +934,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -894,7 +960,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -920,7 +986,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -946,7 +1012,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -972,7 +1038,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -985,9 +1051,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1001,7 +1073,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1020,7 +1092,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1050,7 +1122,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1076,7 +1148,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1102,7 +1174,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1128,7 +1200,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1154,7 +1226,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1180,7 +1252,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1206,7 +1278,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1232,7 +1304,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1258,7 +1330,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1271,104 +1343,123 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5" style="1" customWidth="1"/>
-    <col min="3" max="4" width="19.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
-    <col min="6" max="7" width="19.1719" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="19.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" ht="39" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s" s="3">
+    <row r="2" spans="1:8" ht="39" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" ht="39" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s" s="4">
+    <row r="3" spans="1:8" ht="39" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s" s="4">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s" s="4">
+      <c r="E3" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51180599999999998" footer="0.51180599999999998"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
fix(condo): DOMA-5830 added "isVerified" column for exporting contacts
</commit_message>
<xml_diff>
--- a/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
+++ b/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>{d.i18n.name}</t>
   </si>
@@ -34,6 +34,9 @@
     <t>{d.i18n.role}</t>
   </si>
   <si>
+    <t>{d.i18n.isVerified}</t>
+  </si>
+  <si>
     <t>{d.contacts[i].name}</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t>{d.contacts[i].role}</t>
   </si>
   <si>
+    <t>{d.contacts[i].isVerified}</t>
+  </si>
+  <si>
     <t>{d.contacts[i+1].name}</t>
   </si>
   <si>
@@ -74,13 +80,16 @@
   </si>
   <si>
     <t>{d.contacts[i+1].role}</t>
+  </si>
+  <si>
+    <t>{d.contacts[i+1].isVerified}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -89,15 +98,23 @@
     </font>
     <font>
       <b/>
-      <color theme="1"/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,81 +123,104 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBDC0BF"/>
-        <bgColor rgb="FFBDC0BF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFAFB3B2"/>
+        <bgColor rgb="FFAFB3B2"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border/>
     <border>
       <left style="thin">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FF949494"/>
       </left>
       <right style="thin">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FF949494"/>
       </right>
       <top style="thin">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FF949494"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FFA5A5A5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF303030"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FF949494"/>
       </left>
       <right style="thin">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FF949494"/>
       </right>
+      <top style="thin">
+        <color rgb="FF303030"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FF949494"/>
       </bottom>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF949494"/>
+      </left>
       <right style="thin">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FF949494"/>
       </right>
+      <top style="thin">
+        <color rgb="FF949494"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FF949494"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9A9A9A"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF949494"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9A9A9A"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9A9A9A"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9A9A9A"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9A9A9A"/>
       </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -399,83 +439,163 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.5"/>
-    <col customWidth="1" min="2" max="2" width="30.88"/>
-    <col customWidth="1" min="3" max="3" width="26.0"/>
-    <col customWidth="1" min="4" max="4" width="23.63"/>
-    <col customWidth="1" min="5" max="5" width="18.38"/>
-    <col customWidth="1" min="6" max="6" width="21.13"/>
-    <col customWidth="1" min="7" max="7" width="23.13"/>
+    <col customWidth="1" min="1" max="1" width="30.38"/>
+    <col customWidth="1" min="2" max="2" width="30.5"/>
+    <col customWidth="1" min="3" max="3" width="25.63"/>
+    <col customWidth="1" min="4" max="4" width="23.75"/>
+    <col customWidth="1" min="5" max="5" width="18.88"/>
+    <col customWidth="1" min="6" max="6" width="20.75"/>
+    <col customWidth="1" min="7" max="7" width="21.88"/>
+    <col customWidth="1" min="8" max="8" width="21.25"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
fix(condo): DOMA-10686 Fix export drops
</commit_message>
<xml_diff>
--- a/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
+++ b/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
@@ -1,12 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28308"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5C53772-F02F-4A52-9ADB-082714E22FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="{d.i18n.sheetName}" sheetId="1" r:id="rId4"/>
+    <sheet name="{d.i18n.sheetName}" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -88,30 +108,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -119,7 +133,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -128,8 +142,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
-    <border/>
+  <borders count="4">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF949494"/>
@@ -143,6 +163,7 @@
       <bottom style="thin">
         <color rgb="FF303030"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -157,6 +178,7 @@
       <bottom style="thin">
         <color rgb="FF949494"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -171,72 +193,39 @@
       <bottom style="thin">
         <color rgb="FF949494"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF949494"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -426,30 +415,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.38"/>
-    <col customWidth="1" min="2" max="2" width="30.5"/>
-    <col customWidth="1" min="3" max="3" width="25.63"/>
-    <col customWidth="1" min="4" max="4" width="23.75"/>
-    <col customWidth="1" min="5" max="5" width="18.88"/>
-    <col customWidth="1" min="6" max="6" width="20.75"/>
-    <col customWidth="1" min="7" max="7" width="21.88"/>
-    <col customWidth="1" min="8" max="8" width="21.25"/>
+    <col min="1" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -501,7 +494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -523,81 +516,11 @@
       <c r="G3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(condo): DOMA-10686 fix export drops (#5490)
* fix(condo): DOMA-10686 Fix export drops

* fix(condo): DOMA-10686 fixed utils for excel tables test
</commit_message>
<xml_diff>
--- a/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
+++ b/apps/condo/domains/contact/templates/ContactsExportTemplate.xlsx
@@ -1,12 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28308"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5C53772-F02F-4A52-9ADB-082714E22FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="{d.i18n.sheetName}" sheetId="1" r:id="rId4"/>
+    <sheet name="{d.i18n.sheetName}" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -88,30 +108,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -119,7 +133,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -128,8 +142,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
-    <border/>
+  <borders count="4">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF949494"/>
@@ -143,6 +163,7 @@
       <bottom style="thin">
         <color rgb="FF303030"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -157,6 +178,7 @@
       <bottom style="thin">
         <color rgb="FF949494"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -171,72 +193,39 @@
       <bottom style="thin">
         <color rgb="FF949494"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF949494"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF9A9A9A"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF9A9A9A"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9A9A9A"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9A9A9A"/>
-      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -426,30 +415,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.38"/>
-    <col customWidth="1" min="2" max="2" width="30.5"/>
-    <col customWidth="1" min="3" max="3" width="25.63"/>
-    <col customWidth="1" min="4" max="4" width="23.75"/>
-    <col customWidth="1" min="5" max="5" width="18.88"/>
-    <col customWidth="1" min="6" max="6" width="20.75"/>
-    <col customWidth="1" min="7" max="7" width="21.88"/>
-    <col customWidth="1" min="8" max="8" width="21.25"/>
+    <col min="1" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -501,7 +494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -523,81 +516,11 @@
       <c r="G3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>